<commit_message>
Actualizado MatrizMathTest. Actualizadas métricas y agregado el análisis de rendimiento.
</commit_message>
<xml_diff>
--- a/practica2/trunk/TDAs/doc/analisisRendimiento/AnalisisRendimiento.xlsx
+++ b/practica2/trunk/TDAs/doc/analisisRendimiento/AnalisisRendimiento.xlsx
@@ -1,23 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Dimensión</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Tiempo promedio (ns)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.0000E+00"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -25,16 +40,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -42,23 +77,861 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-AR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="144"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="44"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Tiempo promedio en función de la Dimensión</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tiempo promedio (ns)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:name>O(n^4)</c:name>
+            <c:spPr>
+              <a:ln w="22225">
+                <a:solidFill>
+                  <a:srgbClr val="92D050"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="4"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000E+00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>353198.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1025100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8799496.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64689000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>260610000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1770100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6478300000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17439000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26590000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>56425000000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>141620000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="40468480"/>
+        <c:axId val="40462592"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="40468480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Dimensión del Sistema</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="40462592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="40462592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Tiempo</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0000E+00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="40468480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-AR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="145"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="45"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Error en función de la Dimensión</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja1!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$C$2:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000E+00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>5.1604999999999997E-16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9167999999999999E-15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3510000000000001E-14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0546000000000005E-14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.4444999999999997E-14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5148E-12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4563E-12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.1858E-13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3832E-12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.6200000000000001E-12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.6115999999999999E-12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="65985920"/>
+        <c:axId val="66388736"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="65985920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Dimensión del Sistema</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="66388736"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="66388736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Error</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0000E+00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="65985920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>14286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="1 Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>438149</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>200024</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="2 Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.16315</cdr:x>
+      <cdr:y>0.62</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.8967</cdr:x>
+      <cdr:y>0.62029</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="3" name="2 Conector recto"/>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipV="1">
+          <a:off x="1083129" y="2952750"/>
+          <a:ext cx="4869997" cy="1361"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="sysDot"/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -343,37 +1216,234 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3">
+        <v>353198.5</v>
+      </c>
+      <c r="C2" s="4">
+        <v>5.1604999999999997E-16</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>10</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1025100</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1.9167999999999999E-15</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>50</v>
+      </c>
+      <c r="B4" s="6">
+        <v>8799496.5</v>
+      </c>
+      <c r="C4" s="7">
+        <v>3.3510000000000001E-14</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>100</v>
+      </c>
+      <c r="B5" s="6">
+        <v>64689000</v>
+      </c>
+      <c r="C5" s="7">
+        <v>6.0546000000000005E-14</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>150</v>
+      </c>
+      <c r="B6" s="6">
+        <v>260610000</v>
+      </c>
+      <c r="C6" s="7">
+        <v>6.4444999999999997E-14</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>250</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1770100000</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1.5148E-12</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>350</v>
+      </c>
+      <c r="B8" s="6">
+        <v>6478300000</v>
+      </c>
+      <c r="C8" s="7">
+        <v>1.4563E-12</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>450</v>
+      </c>
+      <c r="B9" s="6">
+        <v>17439000000</v>
+      </c>
+      <c r="C9" s="7">
+        <v>5.1858E-13</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>500</v>
+      </c>
+      <c r="B10" s="6">
+        <v>26590000000</v>
+      </c>
+      <c r="C10" s="7">
+        <v>1.3832E-12</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>600</v>
+      </c>
+      <c r="B11" s="6">
+        <v>56425000000</v>
+      </c>
+      <c r="C11" s="7">
+        <v>2.6200000000000001E-12</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
+        <v>700</v>
+      </c>
+      <c r="B12" s="9">
+        <v>141620000000</v>
+      </c>
+      <c r="C12" s="10">
+        <v>2.6115999999999999E-12</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Realizados los cambios pedidos en SEL: error y vector solución como miembros de SistemaLinealDeEcuaciones. En consecuencia se actualizaron las clases ubicadas en ar.edu.unlam.programacion3.practica2.tda.sel.util.*. Se actualizó al mismo tiempo la documentación del análisis de rendimiento. Se actualizó también por consecuencia de las modificaciones en SistemaLinealDeEcuaciones, las clases MatrizCuadrada y MatrizInvertible (por un tema de constructores).
</commit_message>
<xml_diff>
--- a/practica2/trunk/TDAs/doc/analisisRendimiento/AnalisisRendimiento.xlsx
+++ b/practica2/trunk/TDAs/doc/analisisRendimiento/AnalisisRendimiento.xlsx
@@ -22,7 +22,7 @@
     <t>Error</t>
   </si>
   <si>
-    <t>Tiempo promedio (ns)</t>
+    <t>Tiempo promedio (ms)</t>
   </si>
 </sst>
 </file>
@@ -30,7 +30,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.0000E+00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -69,7 +69,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -174,10 +174,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -187,10 +187,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -200,98 +200,44 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -356,7 +302,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Tiempo promedio (ns)</c:v>
+                  <c:v>Tiempo promedio (ms)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -367,16 +313,20 @@
             </a:ln>
           </c:spPr>
           <c:trendline>
-            <c:name>O(n^4)</c:name>
+            <c:name>O(n^3)</c:name>
             <c:spPr>
-              <a:ln w="22225">
+              <a:ln w="25400" cmpd="sng">
                 <a:solidFill>
-                  <a:srgbClr val="92D050"/>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
                 </a:solidFill>
+                <a:prstDash val="sysDash"/>
               </a:ln>
             </c:spPr>
             <c:trendlineType val="poly"/>
-            <c:order val="4"/>
+            <c:order val="3"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -386,10 +336,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$12</c:f>
+              <c:f>Hoja1!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -422,48 +372,66 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$B$2:$B$12</c:f>
+              <c:f>Hoja1!$B$2:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>0.0000E+00</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>353198.5</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1025100</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8799496.5</c:v>
+                  <c:v>3.3333333333333299</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>64689000</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>260610000</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1770100000</c:v>
+                  <c:v>145.333333333333</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6478300000</c:v>
+                  <c:v>513</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17439000000</c:v>
+                  <c:v>1222.3333333333301</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26590000000</c:v>
+                  <c:v>1789</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>56425000000</c:v>
+                  <c:v>3436.6666666666601</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>141620000000</c:v>
+                  <c:v>7352</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10365.333333333299</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16333.333333333299</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>23145</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -478,11 +446,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="40468480"/>
-        <c:axId val="40462592"/>
+        <c:axId val="119565312"/>
+        <c:axId val="119600256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="40468480"/>
+        <c:axId val="119565312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -512,12 +480,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40462592"/>
+        <c:crossAx val="119600256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="40462592"/>
+        <c:axId val="119600256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -547,7 +515,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40468480"/>
+        <c:crossAx val="119565312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -631,10 +599,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$12</c:f>
+              <c:f>Hoja1!$A$2:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -667,48 +635,60 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$C$2:$C$12</c:f>
+              <c:f>Hoja1!$C$2:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>0.0000E+00</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>5.1604999999999997E-16</c:v>
+                  <c:v>1.9456934202437099E-15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9167999999999999E-15</c:v>
+                  <c:v>2.77149060864267E-15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.3510000000000001E-14</c:v>
+                  <c:v>1.5557172347453501E-13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0546000000000005E-14</c:v>
+                  <c:v>5.0536729344049599E-14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.4444999999999997E-14</c:v>
+                  <c:v>7.3366739577925797E-13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5148E-12</c:v>
+                  <c:v>4.0540499419791701E-13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4563E-12</c:v>
+                  <c:v>2.0674894310851301E-12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.1858E-13</c:v>
+                  <c:v>1.33253241820042E-12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.3832E-12</c:v>
+                  <c:v>6.9590545336786103E-13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.6200000000000001E-12</c:v>
+                  <c:v>3.0422012869607401E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.6115999999999999E-12</c:v>
+                  <c:v>1.2903267584393201E-12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.0716464909443998E-12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.8596923148416803E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -723,11 +703,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="65985920"/>
-        <c:axId val="66388736"/>
+        <c:axId val="120358400"/>
+        <c:axId val="120360320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="65985920"/>
+        <c:axId val="120358400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -757,7 +737,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66388736"/>
+        <c:crossAx val="120360320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -765,7 +745,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66388736"/>
+        <c:axId val="120360320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -795,7 +775,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65985920"/>
+        <c:crossAx val="120358400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -830,7 +810,7 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>19049</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -854,13 +834,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>438149</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>200024</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -887,12 +867,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.16315</cdr:x>
-      <cdr:y>0.62</cdr:y>
+      <cdr:x>0.16458</cdr:x>
+      <cdr:y>0.708</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.8967</cdr:x>
-      <cdr:y>0.62029</cdr:y>
+      <cdr:x>0.89813</cdr:x>
+      <cdr:y>0.70829</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
@@ -901,8 +881,8 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipV="1">
-          <a:off x="1083129" y="2952750"/>
-          <a:ext cx="4869997" cy="1361"/>
+          <a:off x="1092666" y="3371850"/>
+          <a:ext cx="4869983" cy="1381"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
@@ -1217,10 +1197,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C15" sqref="A1:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,14 +1211,14 @@
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1247,199 +1227,237 @@
         <v>5</v>
       </c>
       <c r="B2" s="3">
-        <v>353198.5</v>
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C2" s="4">
-        <v>5.1604999999999997E-16</v>
+        <v>1.9456934202437099E-15</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="2">
         <v>10</v>
       </c>
-      <c r="B3" s="6">
-        <v>1025100</v>
-      </c>
-      <c r="C3" s="7">
-        <v>1.9167999999999999E-15</v>
+      <c r="B3" s="3">
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2.77149060864267E-15</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="2">
         <v>50</v>
       </c>
-      <c r="B4" s="6">
-        <v>8799496.5</v>
-      </c>
-      <c r="C4" s="7">
-        <v>3.3510000000000001E-14</v>
+      <c r="B4" s="3">
+        <v>3.3333333333333299</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1.5557172347453501E-13</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="2">
         <v>100</v>
       </c>
-      <c r="B5" s="6">
-        <v>64689000</v>
-      </c>
-      <c r="C5" s="7">
-        <v>6.0546000000000005E-14</v>
+      <c r="B5" s="3">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4">
+        <v>5.0536729344049599E-14</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="2">
         <v>150</v>
       </c>
-      <c r="B6" s="6">
-        <v>260610000</v>
-      </c>
-      <c r="C6" s="7">
-        <v>6.4444999999999997E-14</v>
+      <c r="B6" s="3">
+        <v>25</v>
+      </c>
+      <c r="C6" s="4">
+        <v>7.3366739577925797E-13</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="2">
         <v>250</v>
       </c>
-      <c r="B7" s="6">
-        <v>1770100000</v>
-      </c>
-      <c r="C7" s="7">
-        <v>1.5148E-12</v>
+      <c r="B7" s="3">
+        <v>145.333333333333</v>
+      </c>
+      <c r="C7" s="4">
+        <v>4.0540499419791701E-13</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="2">
         <v>350</v>
       </c>
-      <c r="B8" s="6">
-        <v>6478300000</v>
-      </c>
-      <c r="C8" s="7">
-        <v>1.4563E-12</v>
+      <c r="B8" s="3">
+        <v>513</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2.0674894310851301E-12</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="2">
         <v>450</v>
       </c>
-      <c r="B9" s="6">
-        <v>17439000000</v>
-      </c>
-      <c r="C9" s="7">
-        <v>5.1858E-13</v>
+      <c r="B9" s="3">
+        <v>1222.3333333333301</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1.33253241820042E-12</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="2">
         <v>500</v>
       </c>
-      <c r="B10" s="6">
-        <v>26590000000</v>
-      </c>
-      <c r="C10" s="7">
-        <v>1.3832E-12</v>
+      <c r="B10" s="3">
+        <v>1789</v>
+      </c>
+      <c r="C10" s="4">
+        <v>6.9590545336786103E-13</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="2">
         <v>600</v>
       </c>
-      <c r="B11" s="6">
-        <v>56425000000</v>
-      </c>
-      <c r="C11" s="7">
-        <v>2.6200000000000001E-12</v>
+      <c r="B11" s="3">
+        <v>3436.6666666666601</v>
+      </c>
+      <c r="C11" s="4">
+        <v>3.0422012869607401E-12</v>
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>700</v>
       </c>
-      <c r="B12" s="9">
-        <v>141620000000</v>
-      </c>
-      <c r="C12" s="10">
-        <v>2.6115999999999999E-12</v>
+      <c r="B12" s="3">
+        <v>7352</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1.2903267584393201E-12</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="A13" s="2">
+        <v>800</v>
+      </c>
+      <c r="B13" s="3">
+        <v>10365.333333333299</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2.0716464909443998E-12</v>
+      </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="A14" s="2">
+        <v>900</v>
+      </c>
+      <c r="B14" s="3">
+        <v>16333.333333333299</v>
+      </c>
+      <c r="C14" s="4">
+        <v>3.8596923148416803E-12</v>
+      </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>1000</v>
+      </c>
+      <c r="B15" s="6">
+        <v>23145</v>
+      </c>
+      <c r="C15" s="7">
+        <v>2.7455201241426401E-11</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>